<commit_message>
partly done with task3
</commit_message>
<xml_diff>
--- a/String_Vibration/M12_Saitenschwingung.xlsx
+++ b/String_Vibration/M12_Saitenschwingung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huyenanh/git_repos/MB14_Classical_mechanics/String_Vibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6799C49-943D-E348-AFA9-B821AE7F6439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E47619-BBED-2749-B1C0-1EB2266D14F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="980" windowWidth="27960" windowHeight="17440" activeTab="1" xr2:uid="{5CF1168E-F7FF-FA41-9351-CBA8D53876DF}"/>
+    <workbookView xWindow="1820" yWindow="980" windowWidth="27960" windowHeight="17440" activeTab="3" xr2:uid="{5CF1168E-F7FF-FA41-9351-CBA8D53876DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Messunsicherheiten" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>-</t>
   </si>
@@ -213,6 +213,30 @@
       <t xml:space="preserve"> in Hz</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri-Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri-Light"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> in Hz</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -525,7 +549,7 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{883CCE7F-A5D3-F34F-BEBA-C1C1F49031CC}" name="fn in Hz" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{883CCE7F-A5D3-F34F-BEBA-C1C1F49031CC}" name="f1 in Hz" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{93CF3EED-9FE8-054A-8B51-40D6DD880E41}" name="n" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{AE73870D-16F5-4849-98D8-F59DEACCC4F5}" name="L in m" dataDxfId="12"/>
     <tableColumn id="4" xr3:uid="{855713B1-F147-7F47-98BC-C4F7A9B61560}" name="M in kg" dataDxfId="11"/>
@@ -896,7 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3082E1-7E34-4048-8DA0-CFD18FE20702}">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="D19" sqref="D19:D23"/>
     </sheetView>
   </sheetViews>
@@ -1142,7 +1166,7 @@
   <dimension ref="A2:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="B5" sqref="B5:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1555,8 +1579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F492D1-66B2-CA4D-8806-FC125DF2E804}">
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1574,7 +1598,7 @@
     </row>
     <row r="4" spans="1:5" ht="17">
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -1588,7 +1612,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="B5" s="2">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -1602,7 +1626,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="B6" s="2">
-        <v>0</v>
+        <v>325</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1616,7 +1640,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="2">
-        <v>0</v>
+        <v>489</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -1630,7 +1654,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="B8" s="2">
-        <v>0</v>
+        <v>654</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -1644,7 +1668,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="B9" s="2">
-        <v>0</v>
+        <v>818</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -1658,7 +1682,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="B10" s="2">
-        <v>0</v>
+        <v>984</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -1672,7 +1696,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="B11" s="2">
-        <v>0</v>
+        <v>1150</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -1686,7 +1710,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="B12" s="2">
-        <v>0</v>
+        <v>1314</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -1700,7 +1724,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="2">
-        <v>0</v>
+        <v>1479</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -1714,7 +1738,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="B14" s="2">
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
fit is not right
</commit_message>
<xml_diff>
--- a/String_Vibration/M12_Saitenschwingung.xlsx
+++ b/String_Vibration/M12_Saitenschwingung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huyenanh/git_repos/MB14_Classical_mechanics/String_Vibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0AC97C-8124-6A40-8754-CD23136F7F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF185DB-17EA-B44E-B2CF-BEEA451A1F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="980" windowWidth="27960" windowHeight="17440" activeTab="2" xr2:uid="{5CF1168E-F7FF-FA41-9351-CBA8D53876DF}"/>
+    <workbookView xWindow="1820" yWindow="980" windowWidth="27960" windowHeight="17440" activeTab="4" xr2:uid="{5CF1168E-F7FF-FA41-9351-CBA8D53876DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Messunsicherheiten" sheetId="5" r:id="rId1"/>
@@ -690,7 +690,7 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0066170D-1124-304E-A978-89197B531952}" name="fn in Hz" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{0066170D-1124-304E-A978-89197B531952}" name="f1 in Hz" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{C5DA23EB-EF7B-2B4C-AF0D-D6D46A50A464}" name="n" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{56E5D647-44AE-3C46-8156-771249AAB216}" name="L in m" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{9348716A-C584-1847-B703-34EDE93B292E}" name="M in kg" dataDxfId="2"/>
@@ -1356,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD34FA5D-5D56-3246-B0BE-0A30FA4FD4B9}">
   <dimension ref="A2:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+    <sheetView zoomScale="113" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2120,8 +2120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5856E6C-5E8C-6A41-A8A7-A9E5D2BE7E03}">
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="200" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2140,7 +2140,7 @@
     </row>
     <row r="4" spans="1:7" ht="17">
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
the sloooope is still wrooong
</commit_message>
<xml_diff>
--- a/String_Vibration/M12_Saitenschwingung.xlsx
+++ b/String_Vibration/M12_Saitenschwingung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huyenanh/git_repos/MB14_Classical_mechanics/String_Vibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF185DB-17EA-B44E-B2CF-BEEA451A1F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD492B1-5112-6E4D-A6B6-6A4B3D43895D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1820" yWindow="980" windowWidth="27960" windowHeight="17440" activeTab="4" xr2:uid="{5CF1168E-F7FF-FA41-9351-CBA8D53876DF}"/>
   </bookViews>
@@ -2118,10 +2118,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5856E6C-5E8C-6A41-A8A7-A9E5D2BE7E03}">
-  <dimension ref="A2:G12"/>
+  <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="200" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2130,7 +2130,7 @@
     <col min="6" max="6" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17">
+    <row r="4" spans="1:8" ht="17">
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2157,8 +2157,9 @@
       <c r="G4" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="32">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="32">
       <c r="B5" s="7">
         <v>46.08</v>
       </c>
@@ -2178,8 +2179,12 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>9.3490000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="32">
+      <c r="H5" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>3.0576134484267303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="32">
       <c r="B6" s="7">
         <v>51.18</v>
       </c>
@@ -2199,8 +2204,12 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>12.292</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="32">
+      <c r="H6" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>3.5059948659403366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="32">
       <c r="B7" s="7">
         <v>57.05</v>
       </c>
@@ -2220,8 +2229,12 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>15.234999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="32">
+      <c r="H7" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>3.9032038122547483</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="32">
       <c r="B8" s="7">
         <v>64.5</v>
       </c>
@@ -2241,8 +2254,12 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>18.178000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="32">
+      <c r="H8" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>4.2635665821000144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="32">
       <c r="B9" s="7">
         <v>67.31</v>
       </c>
@@ -2262,8 +2279,12 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>21.121000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="32">
+      <c r="H9" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>4.5957589144775648</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="32">
       <c r="B10" s="7">
         <v>71.38</v>
       </c>
@@ -2283,8 +2304,12 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>24.064</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="32">
+      <c r="H10" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>4.9055071093618849</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="32">
       <c r="B11" s="7">
         <v>79.84</v>
       </c>
@@ -2304,8 +2329,12 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>27.007000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="32">
+      <c r="H11" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>5.1968259543686859</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="32">
       <c r="B12" s="7">
         <v>81.37</v>
       </c>
@@ -2324,6 +2353,10 @@
       <c r="G12" s="7">
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>29.95</v>
+      </c>
+      <c r="H12" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>5.472659317004851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finally found the issue in task4
</commit_message>
<xml_diff>
--- a/String_Vibration/M12_Saitenschwingung.xlsx
+++ b/String_Vibration/M12_Saitenschwingung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huyenanh/git_repos/MB14_Classical_mechanics/String_Vibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B341C828-E7E5-EF4F-8B32-D3C9BD0F415F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F94F7D6-42DE-9640-AF9D-52CB2A047DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="980" windowWidth="27960" windowHeight="17440" activeTab="2" xr2:uid="{5CF1168E-F7FF-FA41-9351-CBA8D53876DF}"/>
+    <workbookView xWindow="1820" yWindow="980" windowWidth="27960" windowHeight="17440" activeTab="4" xr2:uid="{5CF1168E-F7FF-FA41-9351-CBA8D53876DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Messunsicherheiten" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>-</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>F0 in N</t>
+  </si>
+  <si>
+    <t>sqrt(F0) in sqrt(N)</t>
   </si>
 </sst>
 </file>
@@ -392,7 +395,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="49">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -560,7 +567,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9799FCC7-E3CB-F147-95E4-7DBD94498F82}" name="Table1" displayName="Table1" ref="B4:F13" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9799FCC7-E3CB-F147-95E4-7DBD94498F82}" name="Table1" displayName="Table1" ref="B4:F13" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="B4:F13" xr:uid="{9799FCC7-E3CB-F147-95E4-7DBD94498F82}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -569,11 +576,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{49A74B27-AB55-2C45-B404-17BFD5862C1B}" name="fn in Hz" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{DF3E784A-D43A-9144-B675-D2303F2C1901}" name="n" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{466F7D5D-012C-4540-8451-0B7818BBDDE3}" name="L in m" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{41824933-9B57-9B46-ACB9-4188D316CD4C}" name="M in kg" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{841017D9-1A04-F64D-AD81-8D29A597C135}" name="F0 in N" dataDxfId="41">
+    <tableColumn id="1" xr3:uid="{49A74B27-AB55-2C45-B404-17BFD5862C1B}" name="fn in Hz" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{DF3E784A-D43A-9144-B675-D2303F2C1901}" name="n" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{466F7D5D-012C-4540-8451-0B7818BBDDE3}" name="L in m" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{41824933-9B57-9B46-ACB9-4188D316CD4C}" name="M in kg" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{841017D9-1A04-F64D-AD81-8D29A597C135}" name="F0 in N" dataDxfId="42">
       <calculatedColumnFormula>(Table1[[#This Row],[M in kg]]*9.81) + 0.52</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -582,23 +589,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35855598-C0B3-7F4B-BDAC-42C05A38633F}" name="Table2" displayName="Table2" ref="B18:D23" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35855598-C0B3-7F4B-BDAC-42C05A38633F}" name="Table2" displayName="Table2" ref="B18:D23" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="B18:D23" xr:uid="{35855598-C0B3-7F4B-BDAC-42C05A38633F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3C67841A-ACBD-AB40-A2C6-C116DFD040B2}" name="fn in Hz" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{8D38A66A-AA02-5541-A3B7-505B3C69ABF7}" name="n" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{E625F38D-893B-B048-87F4-0DA04C5B919A}" name="x(Knoten) in m" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{3C67841A-ACBD-AB40-A2C6-C116DFD040B2}" name="fn in Hz" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{8D38A66A-AA02-5541-A3B7-505B3C69ABF7}" name="n" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{E625F38D-893B-B048-87F4-0DA04C5B919A}" name="x(Knoten) in m" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CA1F67FA-AF48-DF4D-8698-4688D7300BFF}" name="Table14" displayName="Table14" ref="B4:F13" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CA1F67FA-AF48-DF4D-8698-4688D7300BFF}" name="Table14" displayName="Table14" ref="B4:F13" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="B4:F13" xr:uid="{CA1F67FA-AF48-DF4D-8698-4688D7300BFF}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -607,18 +614,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5CE74821-3CA7-7F41-A340-50A88F078663}" name="fn in Hz" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{11E5B966-F006-FE4E-A38C-4CB8760C2584}" name="n" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{A3AA1ADC-023E-7448-89E7-BDAD3122080D}" name="L in m" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{9D89E33D-81D5-774C-AFC6-7804FDB9433F}" name="M in kg" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{5B784C43-18D6-D149-95D1-AE5F2038D4B6}" name="F0 in N" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{5CE74821-3CA7-7F41-A340-50A88F078663}" name="fn in Hz" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{11E5B966-F006-FE4E-A38C-4CB8760C2584}" name="n" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{A3AA1ADC-023E-7448-89E7-BDAD3122080D}" name="L in m" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{9D89E33D-81D5-774C-AFC6-7804FDB9433F}" name="M in kg" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{5B784C43-18D6-D149-95D1-AE5F2038D4B6}" name="F0 in N" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{699B8C0F-5E50-9D43-B724-1EE48FFE9DF6}" name="Table15" displayName="Table15" ref="H4:L13" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{699B8C0F-5E50-9D43-B724-1EE48FFE9DF6}" name="Table15" displayName="Table15" ref="H4:L13" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="H4:L13" xr:uid="{699B8C0F-5E50-9D43-B724-1EE48FFE9DF6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -627,18 +634,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3A1A20D1-7D08-5443-BA89-3DD06B4CC92B}" name="fn in Hz" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{1DC18D2B-10DD-984F-B961-03184B763CD8}" name="n" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{BA959F47-D3A0-AC46-BB54-364453A84FA2}" name="L in m" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{6E8C8822-E539-8F41-A48F-F06B5F45AD30}" name="M in kg" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{EDBD39CE-68F2-4747-A67A-03E7CE008D80}" name="F0 in N" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{3A1A20D1-7D08-5443-BA89-3DD06B4CC92B}" name="fn in Hz" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{1DC18D2B-10DD-984F-B961-03184B763CD8}" name="n" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{BA959F47-D3A0-AC46-BB54-364453A84FA2}" name="L in m" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{6E8C8822-E539-8F41-A48F-F06B5F45AD30}" name="M in kg" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{EDBD39CE-68F2-4747-A67A-03E7CE008D80}" name="F0 in N" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{28BFDA7B-DE79-CD46-80BD-B13681D24FB7}" name="Table16" displayName="Table16" ref="N4:R13" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{28BFDA7B-DE79-CD46-80BD-B13681D24FB7}" name="Table16" displayName="Table16" ref="N4:R13" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="N4:R13" xr:uid="{28BFDA7B-DE79-CD46-80BD-B13681D24FB7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -647,18 +654,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3B183D1C-C7B6-E242-B3D2-D8DAD6342E17}" name="fn in Hz" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{2E41B9D4-B8E9-4544-A5DF-91E2D5408375}" name="n" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{A82D5EEF-720C-4749-B5D8-4BE67E617275}" name="L in m" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{94347ED6-07C6-C342-8921-F2424497039E}" name="M in kg" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{21ABC2FB-7D06-074E-B917-F7A131D058F4}" name="F0 in N" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{3B183D1C-C7B6-E242-B3D2-D8DAD6342E17}" name="fn in Hz" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{2E41B9D4-B8E9-4544-A5DF-91E2D5408375}" name="n" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{A82D5EEF-720C-4749-B5D8-4BE67E617275}" name="L in m" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{94347ED6-07C6-C342-8921-F2424497039E}" name="M in kg" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{21ABC2FB-7D06-074E-B917-F7A131D058F4}" name="F0 in N" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A4220B27-9BE7-C348-8CFD-34363984CFF3}" name="Table17" displayName="Table17" ref="B4:F14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A4220B27-9BE7-C348-8CFD-34363984CFF3}" name="Table17" displayName="Table17" ref="B4:F14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="B4:F14" xr:uid="{A4220B27-9BE7-C348-8CFD-34363984CFF3}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -667,11 +674,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{883CCE7F-A5D3-F34F-BEBA-C1C1F49031CC}" name="f1 in Hz" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{93CF3EED-9FE8-054A-8B51-40D6DD880E41}" name="n" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{AE73870D-16F5-4849-98D8-F59DEACCC4F5}" name="L in m" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{855713B1-F147-7F47-98BC-C4F7A9B61560}" name="M in kg" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{D64068DB-E09C-0B43-A632-78B30077CDBD}" name="F0 in N" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{883CCE7F-A5D3-F34F-BEBA-C1C1F49031CC}" name="f1 in Hz" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{93CF3EED-9FE8-054A-8B51-40D6DD880E41}" name="n" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{AE73870D-16F5-4849-98D8-F59DEACCC4F5}" name="L in m" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{855713B1-F147-7F47-98BC-C4F7A9B61560}" name="M in kg" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{D64068DB-E09C-0B43-A632-78B30077CDBD}" name="F0 in N" dataDxfId="9">
       <calculatedColumnFormula>(Table17[[#This Row],[M in kg]]*9.81) + 0.52</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -680,23 +687,27 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{75CF1196-BAD9-E044-9BA3-3DDF21B6BF83}" name="Table18" displayName="Table18" ref="B4:G12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B4:G12" xr:uid="{75CF1196-BAD9-E044-9BA3-3DDF21B6BF83}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{75CF1196-BAD9-E044-9BA3-3DDF21B6BF83}" name="Table18" displayName="Table18" ref="B4:H12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B4:H12" xr:uid="{75CF1196-BAD9-E044-9BA3-3DDF21B6BF83}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0066170D-1124-304E-A978-89197B531952}" name="f1 in Hz" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{C5DA23EB-EF7B-2B4C-AF0D-D6D46A50A464}" name="n" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{56E5D647-44AE-3C46-8156-771249AAB216}" name="L in m" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{9348716A-C584-1847-B703-34EDE93B292E}" name="M in kg" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{15FE26B0-C0F9-794F-95BF-D74B3814F458}" name="Hebelübersetzung" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{CD2C33DF-04EB-AB4F-9798-180CB360BC50}" name="F0 in N" dataDxfId="0">
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{0066170D-1124-304E-A978-89197B531952}" name="f1 in Hz" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{C5DA23EB-EF7B-2B4C-AF0D-D6D46A50A464}" name="n" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{56E5D647-44AE-3C46-8156-771249AAB216}" name="L in m" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{9348716A-C584-1847-B703-34EDE93B292E}" name="M in kg" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{15FE26B0-C0F9-794F-95BF-D74B3814F458}" name="Hebelübersetzung" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{CD2C33DF-04EB-AB4F-9798-180CB360BC50}" name="F0 in N" dataDxfId="1">
       <calculatedColumnFormula>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{B2757821-1127-944D-8B19-FC3E299D58F5}" name="sqrt(F0) in sqrt(N)" dataDxfId="0">
+      <calculatedColumnFormula>SQRT(Table18[[#This Row],[F0 in N]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1356,7 +1367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD34FA5D-5D56-3246-B0BE-0A30FA4FD4B9}">
   <dimension ref="A2:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="113" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -2120,14 +2131,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5856E6C-5E8C-6A41-A8A7-A9E5D2BE7E03}">
   <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="91" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2159,7 +2171,9 @@
       <c r="G4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="32">
       <c r="B5" s="7">
@@ -2181,7 +2195,10 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>9.3490000000000002</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>3.0576134484267303</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="32">
       <c r="B6" s="7">
@@ -2203,7 +2220,10 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>12.292</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>3.5059948659403366</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="32">
       <c r="B7" s="7">
@@ -2225,7 +2245,10 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>15.234999999999999</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>3.9032038122547483</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="32">
       <c r="B8" s="7">
@@ -2247,7 +2270,10 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>18.178000000000001</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>4.2635665821000144</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="32">
       <c r="B9" s="7">
@@ -2269,7 +2295,10 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>21.121000000000002</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>4.5957589144775648</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="32">
       <c r="B10" s="7">
@@ -2291,7 +2320,10 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>24.064</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>4.9055071093618849</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="32">
       <c r="B11" s="7">
@@ -2313,7 +2345,10 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>27.007000000000001</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>5.1968259543686859</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="32">
       <c r="B12" s="7">
@@ -2335,7 +2370,10 @@
         <f>(Table18[[#This Row],[M in kg]]*9.81) + 0.52</f>
         <v>29.95</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7">
+        <f>SQRT(Table18[[#This Row],[F0 in N]])</f>
+        <v>5.472659317004851</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>